<commit_message>
set rainbow road as default song again
</commit_message>
<xml_diff>
--- a/Assets/Resources/Overkill/overkill.xlsx
+++ b/Assets/Resources/Overkill/overkill.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\Songs\992847 RIOT - Overkill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\College\Software - Project 2 COMP313\Rhythm-Road\Assets\Resources\Overkill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F127C0C9-774C-4FDB-BA07-EB96AEE1B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59396B33-8F5D-4B08-B449-AEECBCFD59F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B294" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C300" sqref="C300"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <f t="shared" si="2"/>

</xml_diff>